<commit_message>
- Bei Personen, bei denen das Lehramt fehlt, werden nun auch Gruppen erzeugt, jedoch mit '???' als Platzhalter. Zum Beispiel LAA_???_2020-10 - Code-Optimierung - Bugfixing - Errorhandling
</commit_message>
<xml_diff>
--- a/Beispiel_LAA_ADELE_Erstexport.xlsx
+++ b/Beispiel_LAA_ADELE_Erstexport.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\-= ZfsL =-\Mediengruppe\Logineo NRW\DEV\ADELE_to_LOGINEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05B79623-EA4C-406C-84E4-F47362DBB0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056AA464-BF85-4628-B66F-7F936E69B2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="1890" yWindow="3105" windowWidth="24870" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Beispiel_LAA_ADELE_Erstexport" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1226,10 +1226,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1491,9 +1493,6 @@
       <c r="T2" t="s">
         <v>79</v>
       </c>
-      <c r="X2">
-        <v>8</v>
-      </c>
       <c r="Y2" t="s">
         <v>80</v>
       </c>

</xml_diff>